<commit_message>
helper file to generate C code from XLS file and XLS file comment updates
</commit_message>
<xml_diff>
--- a/Docs/TM4C_controller_pin_specs.xlsx
+++ b/Docs/TM4C_controller_pin_specs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\hardware\CMS_Trigger\6089-103_ATCA_mezz\GitHub\CU_PCB_6089-103\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wittich/src/CU_PCB_6089-103/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D815DC-4857-5547-8023-82C6FC82B00B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="0" windowWidth="7785" windowHeight="435"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="351">
   <si>
     <t>Pin Number</t>
   </si>
@@ -1076,11 +1077,26 @@
   <si>
     <t xml:space="preserve">TM4C_DIP_SW_1: Wired to position #4 of switch SW4, the KU15P DIP SWITCH. A HI level means that the KU15P should be powered; a LO level means that the KU15P should be left unpowered. The pullup on the switch is energized from the VCC_M3V3 source, so it is valid whenever the board has 12V supplied. </t>
   </si>
+  <si>
+    <t>DO NOT PROGRAM</t>
+  </si>
+  <si>
+    <t>JTAG_TDO</t>
+  </si>
+  <si>
+    <t>JTAG_TDI</t>
+  </si>
+  <si>
+    <t>JTAG_TMS</t>
+  </si>
+  <si>
+    <t>JTAG_TCK</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1291,6 +1307,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1326,6 +1359,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1501,48 +1551,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F136"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="H90" sqref="H90"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="J102" sqref="J102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="5" customWidth="1"/>
     <col min="5" max="5" width="34" style="3" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="36.5" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="8"/>
       <c r="B1" s="12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
       <c r="B2" s="12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="12" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>0</v>
       </c>
@@ -1562,7 +1612,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>1</v>
       </c>
@@ -1582,7 +1632,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2</v>
       </c>
@@ -1602,7 +1652,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>3</v>
       </c>
@@ -1622,7 +1672,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>4</v>
       </c>
@@ -1642,7 +1692,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>5</v>
       </c>
@@ -1662,7 +1712,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>6</v>
       </c>
@@ -1682,7 +1732,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <v>7</v>
       </c>
@@ -1699,7 +1749,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>8</v>
       </c>
@@ -1716,7 +1766,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>9</v>
       </c>
@@ -1733,7 +1783,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>10</v>
       </c>
@@ -1750,7 +1800,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>11</v>
       </c>
@@ -1770,7 +1820,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>12</v>
       </c>
@@ -1790,7 +1840,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>13</v>
       </c>
@@ -1810,7 +1860,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>14</v>
       </c>
@@ -1830,7 +1880,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>15</v>
       </c>
@@ -1850,7 +1900,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <v>16</v>
       </c>
@@ -1867,7 +1917,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <v>17</v>
       </c>
@@ -1884,7 +1934,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>18</v>
       </c>
@@ -1904,7 +1954,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>19</v>
       </c>
@@ -1924,7 +1974,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>20</v>
       </c>
@@ -1944,7 +1994,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
         <v>21</v>
       </c>
@@ -1964,7 +2014,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>22</v>
       </c>
@@ -1984,7 +2034,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>23</v>
       </c>
@@ -2004,7 +2054,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>24</v>
       </c>
@@ -2024,7 +2074,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <v>25</v>
       </c>
@@ -2044,7 +2094,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="10">
         <v>26</v>
       </c>
@@ -2061,7 +2111,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
         <v>27</v>
       </c>
@@ -2081,7 +2131,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="10">
         <v>28</v>
       </c>
@@ -2098,7 +2148,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="8">
         <v>29</v>
       </c>
@@ -2118,7 +2168,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <v>30</v>
       </c>
@@ -2138,7 +2188,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <v>31</v>
       </c>
@@ -2158,7 +2208,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="8">
         <v>32</v>
       </c>
@@ -2178,7 +2228,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
         <v>33</v>
       </c>
@@ -2198,7 +2248,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="9">
         <v>34</v>
       </c>
@@ -2218,7 +2268,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="9">
         <v>35</v>
       </c>
@@ -2238,7 +2288,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="9">
         <v>36</v>
       </c>
@@ -2258,7 +2308,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
         <v>37</v>
       </c>
@@ -2278,7 +2328,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="8">
         <v>38</v>
       </c>
@@ -2298,7 +2348,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A47" s="10">
         <v>39</v>
       </c>
@@ -2315,7 +2365,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
         <v>40</v>
       </c>
@@ -2335,7 +2385,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="9">
         <v>41</v>
       </c>
@@ -2355,7 +2405,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <v>42</v>
       </c>
@@ -2375,7 +2425,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
         <v>43</v>
       </c>
@@ -2395,7 +2445,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
         <v>44</v>
       </c>
@@ -2415,7 +2465,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
         <v>45</v>
       </c>
@@ -2435,7 +2485,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
         <v>46</v>
       </c>
@@ -2455,7 +2505,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" s="10">
         <v>47</v>
       </c>
@@ -2472,7 +2522,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="10">
         <v>48</v>
       </c>
@@ -2489,7 +2539,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A57" s="9">
         <v>49</v>
       </c>
@@ -2509,7 +2559,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="9">
         <v>50</v>
       </c>
@@ -2529,7 +2579,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A59" s="9">
         <v>51</v>
       </c>
@@ -2549,7 +2599,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="9">
         <v>52</v>
       </c>
@@ -2569,7 +2619,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A61" s="9">
         <v>53</v>
       </c>
@@ -2589,7 +2639,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="9">
         <v>54</v>
       </c>
@@ -2609,7 +2659,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A63" s="9">
         <v>55</v>
       </c>
@@ -2629,7 +2679,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="9">
         <v>56</v>
       </c>
@@ -2649,7 +2699,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
         <v>57</v>
       </c>
@@ -2669,7 +2719,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="8">
         <v>58</v>
       </c>
@@ -2689,7 +2739,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="8">
         <v>59</v>
       </c>
@@ -2709,7 +2759,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="8">
         <v>60</v>
       </c>
@@ -2729,7 +2779,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="8">
         <v>61</v>
       </c>
@@ -2749,7 +2799,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="8">
         <v>62</v>
       </c>
@@ -2769,7 +2819,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A71" s="10">
         <v>63</v>
       </c>
@@ -2786,7 +2836,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A72" s="10">
         <v>64</v>
       </c>
@@ -2806,7 +2856,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="10">
         <v>65</v>
       </c>
@@ -2826,7 +2876,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A74" s="10">
         <v>66</v>
       </c>
@@ -2846,7 +2896,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A75" s="10">
         <v>67</v>
       </c>
@@ -2866,7 +2916,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A76" s="10">
         <v>68</v>
       </c>
@@ -2883,7 +2933,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A77" s="10">
         <v>69</v>
       </c>
@@ -2900,7 +2950,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A78" s="10">
         <v>70</v>
       </c>
@@ -2920,7 +2970,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A79" s="8">
         <v>71</v>
       </c>
@@ -2940,7 +2990,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A80" s="8">
         <v>72</v>
       </c>
@@ -2960,7 +3010,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A81" s="8">
         <v>73</v>
       </c>
@@ -2980,7 +3030,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="8">
         <v>74</v>
       </c>
@@ -3000,7 +3050,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="8">
         <v>75</v>
       </c>
@@ -3020,7 +3070,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="8">
         <v>76</v>
       </c>
@@ -3040,7 +3090,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="8">
         <v>77</v>
       </c>
@@ -3060,7 +3110,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A86" s="8">
         <v>78</v>
       </c>
@@ -3080,7 +3130,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A87" s="10">
         <v>79</v>
       </c>
@@ -3097,7 +3147,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="10">
         <v>80</v>
       </c>
@@ -3114,7 +3164,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A89" s="8">
         <v>81</v>
       </c>
@@ -3134,7 +3184,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A90" s="8">
         <v>82</v>
       </c>
@@ -3154,7 +3204,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="8">
         <v>83</v>
       </c>
@@ -3174,7 +3224,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="8">
         <v>84</v>
       </c>
@@ -3194,7 +3244,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="8">
         <v>85</v>
       </c>
@@ -3214,7 +3264,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="8">
         <v>86</v>
       </c>
@@ -3234,7 +3284,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A95" s="10">
         <v>87</v>
       </c>
@@ -3251,7 +3301,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="10">
         <v>88</v>
       </c>
@@ -3271,7 +3321,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A97" s="10">
         <v>89</v>
       </c>
@@ -3291,7 +3341,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A98" s="10">
         <v>90</v>
       </c>
@@ -3308,7 +3358,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A99" s="9">
         <v>91</v>
       </c>
@@ -3328,7 +3378,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="9">
         <v>92</v>
       </c>
@@ -3348,7 +3398,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="8">
         <v>93</v>
       </c>
@@ -3368,7 +3418,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="8">
         <v>94</v>
       </c>
@@ -3388,7 +3438,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="9">
         <v>95</v>
       </c>
@@ -3408,7 +3458,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="9">
         <v>96</v>
       </c>
@@ -3428,7 +3478,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A105" s="9">
         <v>97</v>
       </c>
@@ -3444,8 +3494,14 @@
       <c r="E105" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F105" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="G105" s="4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A106" s="9">
         <v>98</v>
       </c>
@@ -3461,8 +3517,14 @@
       <c r="E106" s="3" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F106" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="G106" s="4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A107" s="9">
         <v>99</v>
       </c>
@@ -3478,8 +3540,14 @@
       <c r="E107" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F107" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="G107" s="4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A108" s="9">
         <v>100</v>
       </c>
@@ -3495,8 +3563,14 @@
       <c r="E108" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F108" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="G108" s="4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A109" s="10">
         <v>101</v>
       </c>
@@ -3513,7 +3587,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="8">
         <v>102</v>
       </c>
@@ -3533,7 +3607,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="8">
         <v>103</v>
       </c>
@@ -3553,7 +3627,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A112" s="8">
         <v>104</v>
       </c>
@@ -3573,7 +3647,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A113" s="8">
         <v>105</v>
       </c>
@@ -3593,7 +3667,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A114" s="8">
         <v>106</v>
       </c>
@@ -3613,7 +3687,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="8">
         <v>107</v>
       </c>
@@ -3633,7 +3707,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="8">
         <v>108</v>
       </c>
@@ -3653,7 +3727,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="8">
         <v>109</v>
       </c>
@@ -3673,7 +3747,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="8">
         <v>110</v>
       </c>
@@ -3693,7 +3767,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="8">
         <v>111</v>
       </c>
@@ -3713,7 +3787,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="8">
         <v>112</v>
       </c>
@@ -3733,7 +3807,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A121" s="10">
         <v>113</v>
       </c>
@@ -3750,7 +3824,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="10">
         <v>114</v>
       </c>
@@ -3767,7 +3841,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A123" s="10">
         <v>115</v>
       </c>
@@ -3784,7 +3858,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="8">
         <v>116</v>
       </c>
@@ -3804,7 +3878,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="8">
         <v>117</v>
       </c>
@@ -3824,7 +3898,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="8">
         <v>118</v>
       </c>
@@ -3844,7 +3918,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A127" s="8">
         <v>119</v>
       </c>
@@ -3864,7 +3938,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="11">
         <v>120</v>
       </c>
@@ -3884,7 +3958,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="11">
         <v>121</v>
       </c>
@@ -3904,7 +3978,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A130" s="10">
         <v>122</v>
       </c>
@@ -3921,7 +3995,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="11">
         <v>123</v>
       </c>
@@ -3941,7 +4015,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="11">
         <v>124</v>
       </c>
@@ -3961,7 +4035,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="11">
         <v>125</v>
       </c>
@@ -3981,7 +4055,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="11">
         <v>126</v>
       </c>
@@ -4001,7 +4075,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="11">
         <v>127</v>
       </c>
@@ -4021,7 +4095,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="11">
         <v>128</v>
       </c>
@@ -4042,7 +4116,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A9:F136">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:F136">
     <sortCondition ref="A9:A136"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4050,24 +4124,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>